<commit_message>
added shigela and salmonela
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_fields.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_fields.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="175">
   <si>
     <t>COUNTRY_A</t>
   </si>
@@ -542,6 +542,12 @@
   </si>
   <si>
     <t>LOCAL_SPEC</t>
+  </si>
+  <si>
+    <t>FOS_ND200</t>
+  </si>
+  <si>
+    <t>FOS_NM</t>
   </si>
 </sst>
 </file>
@@ -1349,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FF166"/>
+  <dimension ref="A1:FF168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2839,6 +2845,22 @@
         <v>170</v>
       </c>
     </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finished the summary report with checking pa
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_fields.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_fields.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="179">
   <si>
     <t>COUNTRY_A</t>
   </si>
@@ -548,6 +548,18 @@
   </si>
   <si>
     <t>FOS_NM</t>
+  </si>
+  <si>
+    <t>DOX_ND30</t>
+  </si>
+  <si>
+    <t>DOX_NM</t>
+  </si>
+  <si>
+    <t>SSS_ND200</t>
+  </si>
+  <si>
+    <t>SSS_NM</t>
   </si>
 </sst>
 </file>
@@ -1355,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FF168"/>
+  <dimension ref="A1:FF172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2861,6 +2873,38 @@
         <v>170</v>
       </c>
     </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed .0 on antibiotic disk test
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_fields.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_fields.xlsx
@@ -529,9 +529,6 @@
     <t>GROWTH</t>
   </si>
   <si>
-    <t>MECA</t>
-  </si>
-  <si>
     <t>AMPC</t>
   </si>
   <si>
@@ -560,6 +557,9 @@
   </si>
   <si>
     <t>SSS_NM</t>
+  </si>
+  <si>
+    <t>X_MECA</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FF172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B172" sqref="B172"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>165</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>166</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>166</v>
@@ -1902,7 +1902,7 @@
         <v>38</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1910,7 +1910,7 @@
         <v>39</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1918,7 +1918,7 @@
         <v>40</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1926,7 +1926,7 @@
         <v>41</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1934,7 +1934,7 @@
         <v>42</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1942,7 +1942,7 @@
         <v>43</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1950,7 +1950,7 @@
         <v>44</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1958,7 +1958,7 @@
         <v>45</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1966,7 +1966,7 @@
         <v>46</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,7 +1974,7 @@
         <v>47</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1982,7 +1982,7 @@
         <v>48</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1990,7 +1990,7 @@
         <v>49</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1998,7 +1998,7 @@
         <v>50</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2006,7 +2006,7 @@
         <v>51</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>52</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2022,7 +2022,7 @@
         <v>53</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2030,7 +2030,7 @@
         <v>54</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2038,7 +2038,7 @@
         <v>55</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2046,7 +2046,7 @@
         <v>56</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2054,7 +2054,7 @@
         <v>57</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2062,7 +2062,7 @@
         <v>58</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2070,7 +2070,7 @@
         <v>59</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2078,7 +2078,7 @@
         <v>60</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2086,7 +2086,7 @@
         <v>61</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2094,7 +2094,7 @@
         <v>62</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2102,7 +2102,7 @@
         <v>63</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2110,7 +2110,7 @@
         <v>64</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2118,7 +2118,7 @@
         <v>65</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2126,7 +2126,7 @@
         <v>66</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2134,7 +2134,7 @@
         <v>67</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2142,7 +2142,7 @@
         <v>68</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2150,7 +2150,7 @@
         <v>69</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>70</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2166,7 +2166,7 @@
         <v>71</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2174,7 +2174,7 @@
         <v>72</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2182,7 +2182,7 @@
         <v>73</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2190,7 +2190,7 @@
         <v>74</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2198,7 +2198,7 @@
         <v>75</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2206,7 +2206,7 @@
         <v>76</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2214,7 +2214,7 @@
         <v>77</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2222,7 +2222,7 @@
         <v>78</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
         <v>79</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2238,7 +2238,7 @@
         <v>80</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2246,7 +2246,7 @@
         <v>81</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2254,7 +2254,7 @@
         <v>82</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>83</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2270,7 +2270,7 @@
         <v>84</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2278,7 +2278,7 @@
         <v>85</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2286,7 +2286,7 @@
         <v>86</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2294,7 +2294,7 @@
         <v>87</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2302,7 +2302,7 @@
         <v>88</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2310,7 +2310,7 @@
         <v>89</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
         <v>90</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2326,7 +2326,7 @@
         <v>91</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
         <v>92</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2342,7 +2342,7 @@
         <v>93</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
         <v>94</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2358,7 +2358,7 @@
         <v>95</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2366,7 +2366,7 @@
         <v>96</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2374,7 +2374,7 @@
         <v>97</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2382,7 +2382,7 @@
         <v>98</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2390,7 +2390,7 @@
         <v>99</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2398,7 +2398,7 @@
         <v>100</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2406,7 +2406,7 @@
         <v>101</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2414,7 +2414,7 @@
         <v>102</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2422,7 +2422,7 @@
         <v>103</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
         <v>104</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2438,7 +2438,7 @@
         <v>105</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2446,7 +2446,7 @@
         <v>106</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2454,7 +2454,7 @@
         <v>107</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2462,7 +2462,7 @@
         <v>108</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2470,7 +2470,7 @@
         <v>109</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2478,7 +2478,7 @@
         <v>110</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2486,7 +2486,7 @@
         <v>111</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
         <v>112</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2502,7 +2502,7 @@
         <v>113</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,7 +2510,7 @@
         <v>114</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2518,7 +2518,7 @@
         <v>115</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2526,7 +2526,7 @@
         <v>116</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2534,7 +2534,7 @@
         <v>117</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2542,7 +2542,7 @@
         <v>118</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2550,7 +2550,7 @@
         <v>119</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
         <v>120</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2566,7 +2566,7 @@
         <v>121</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2574,7 +2574,7 @@
         <v>122</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
         <v>123</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2590,7 +2590,7 @@
         <v>124</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2598,7 +2598,7 @@
         <v>125</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2606,7 +2606,7 @@
         <v>126</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,7 +2614,7 @@
         <v>127</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -2622,7 +2622,7 @@
         <v>128</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -2630,7 +2630,7 @@
         <v>129</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
         <v>130</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -2646,7 +2646,7 @@
         <v>131</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -2654,7 +2654,7 @@
         <v>132</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2662,7 +2662,7 @@
         <v>133</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
         <v>134</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -2678,7 +2678,7 @@
         <v>135</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2686,7 +2686,7 @@
         <v>136</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -2694,7 +2694,7 @@
         <v>137</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -2702,7 +2702,7 @@
         <v>138</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -2710,7 +2710,7 @@
         <v>139</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -2718,7 +2718,7 @@
         <v>140</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -2726,7 +2726,7 @@
         <v>141</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -2734,7 +2734,7 @@
         <v>142</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -2742,7 +2742,7 @@
         <v>143</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -2750,7 +2750,7 @@
         <v>144</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -2758,7 +2758,7 @@
         <v>145</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -2766,7 +2766,7 @@
         <v>146</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -2774,7 +2774,7 @@
         <v>147</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -2782,7 +2782,7 @@
         <v>148</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -2790,7 +2790,7 @@
         <v>149</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -2798,7 +2798,7 @@
         <v>150</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -2806,7 +2806,7 @@
         <v>151</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -2814,7 +2814,7 @@
         <v>152</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -2822,7 +2822,7 @@
         <v>153</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -2830,7 +2830,7 @@
         <v>154</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -2838,7 +2838,7 @@
         <v>155</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>156</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -2854,55 +2854,55 @@
         <v>157</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added NM -> NE function and many bug fixes
</commit_message>
<xml_diff>
--- a/whonet/static/whonet_xl/whonet_data_fields.xlsx
+++ b/whonet/static/whonet_xl/whonet_data_fields.xlsx
@@ -9,13 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13125"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13125" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="W2019PHL" sheetId="1" r:id="rId1"/>
+    <sheet name="etest" sheetId="2" r:id="rId2"/>
+    <sheet name="mic" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">W2019PHL!$B$1:$B$166</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">etest!$A$1:$A$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">W2019PHL!$B$1:$B$235</definedName>
     <definedName name="_xlnm.Database">W2019PHL!#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="243">
   <si>
     <t>COUNTRY_A</t>
   </si>
@@ -560,6 +563,198 @@
   </si>
   <si>
     <t>X_MECA</t>
+  </si>
+  <si>
+    <t>AMK_NE</t>
+  </si>
+  <si>
+    <t>AMC_NE</t>
+  </si>
+  <si>
+    <t>AMP_NE</t>
+  </si>
+  <si>
+    <t>SAM_NE</t>
+  </si>
+  <si>
+    <t>AZM_NE</t>
+  </si>
+  <si>
+    <t>ATM_NE</t>
+  </si>
+  <si>
+    <t>CEC_NE</t>
+  </si>
+  <si>
+    <t>MAN_NE</t>
+  </si>
+  <si>
+    <t>CZO_NE</t>
+  </si>
+  <si>
+    <t>FEP_NE</t>
+  </si>
+  <si>
+    <t>CFM_NE</t>
+  </si>
+  <si>
+    <t>CFP_NE</t>
+  </si>
+  <si>
+    <t>CTX_NE</t>
+  </si>
+  <si>
+    <t>FOX_NE</t>
+  </si>
+  <si>
+    <t>CAZ_NE</t>
+  </si>
+  <si>
+    <t>CRO_NE</t>
+  </si>
+  <si>
+    <t>CXM_NE</t>
+  </si>
+  <si>
+    <t>CXA_NE</t>
+  </si>
+  <si>
+    <t>CEP_NE</t>
+  </si>
+  <si>
+    <t>CHL_NE</t>
+  </si>
+  <si>
+    <t>CIP_NE</t>
+  </si>
+  <si>
+    <t>CLR_NE</t>
+  </si>
+  <si>
+    <t>CLI_NE</t>
+  </si>
+  <si>
+    <t>COL_NE</t>
+  </si>
+  <si>
+    <t>SXT_NE</t>
+  </si>
+  <si>
+    <t>DAP_NE</t>
+  </si>
+  <si>
+    <t>DOR_NE</t>
+  </si>
+  <si>
+    <t>ETP_NE</t>
+  </si>
+  <si>
+    <t>ERY_NE</t>
+  </si>
+  <si>
+    <t>GEN_NE</t>
+  </si>
+  <si>
+    <t>GEH_NE</t>
+  </si>
+  <si>
+    <t>IPM_NE</t>
+  </si>
+  <si>
+    <t>KAN_NE</t>
+  </si>
+  <si>
+    <t>LVX_NE</t>
+  </si>
+  <si>
+    <t>LNZ_NE</t>
+  </si>
+  <si>
+    <t>MEM_NE</t>
+  </si>
+  <si>
+    <t>MNO_NE</t>
+  </si>
+  <si>
+    <t>MFX_NE</t>
+  </si>
+  <si>
+    <t>NAL_NE</t>
+  </si>
+  <si>
+    <t>NET_NE</t>
+  </si>
+  <si>
+    <t>NIT_NE</t>
+  </si>
+  <si>
+    <t>NOR_NE</t>
+  </si>
+  <si>
+    <t>NOV_NE</t>
+  </si>
+  <si>
+    <t>OFX_NE</t>
+  </si>
+  <si>
+    <t>OXA_NE</t>
+  </si>
+  <si>
+    <t>PEN_NE</t>
+  </si>
+  <si>
+    <t>PIP_NE</t>
+  </si>
+  <si>
+    <t>TZP_NE</t>
+  </si>
+  <si>
+    <t>POL_NE</t>
+  </si>
+  <si>
+    <t>QDA_NE</t>
+  </si>
+  <si>
+    <t>RIF_NE</t>
+  </si>
+  <si>
+    <t>SPT_NE</t>
+  </si>
+  <si>
+    <t>STR_NE</t>
+  </si>
+  <si>
+    <t>STH_NE</t>
+  </si>
+  <si>
+    <t>TCY_NE</t>
+  </si>
+  <si>
+    <t>TIC_NE</t>
+  </si>
+  <si>
+    <t>TCC_NE</t>
+  </si>
+  <si>
+    <t>TGC_NE</t>
+  </si>
+  <si>
+    <t>TOB_NE</t>
+  </si>
+  <si>
+    <t>VAN_NE</t>
+  </si>
+  <si>
+    <t>FOS_NE</t>
+  </si>
+  <si>
+    <t>DOX_NE</t>
+  </si>
+  <si>
+    <t>SSS_NE</t>
+  </si>
+  <si>
+    <t>ABX_ETEST</t>
   </si>
 </sst>
 </file>
@@ -1367,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FF172"/>
+  <dimension ref="A1:FF235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2905,6 +3100,1570 @@
         <v>169</v>
       </c>
     </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:B235"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>